<commit_message>
Toqueteo en reunion con cristina
</commit_message>
<xml_diff>
--- a/resultados/PCA_factor_loadings.xlsx
+++ b/resultados/PCA_factor_loadings.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\collf\Documents\GitHub\TFM-Ortiguilla\resultados\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{C2693124-C0DC-4BF3-AA18-8EE49808153D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{397A8762-BD15-4D4D-824B-ADD1B8312D4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCA_factor_loadings sin DTD" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
@@ -109,10 +109,10 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0%"/>
-    <numFmt numFmtId="171" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
@@ -639,45 +639,43 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="18" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="171" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="18" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="171" fontId="19" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -744,16 +742,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>44450</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>139700</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>203200</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -783,7 +781,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="800100" y="6769100"/>
+          <a:off x="3359150" y="7023100"/>
           <a:ext cx="3892550" cy="2959100"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1102,11 +1100,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:L36"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="G50" sqref="G50"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="L47" sqref="L47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1679,487 +1677,487 @@
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B20" s="8" t="s">
+      <c r="B20" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="8">
         <v>3.4647221226171099</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="8">
         <v>2.0097472725941801</v>
       </c>
-      <c r="E20" s="9">
+      <c r="E20" s="8">
         <v>1.7383263336519901</v>
       </c>
-      <c r="F20" s="9">
+      <c r="F20" s="8">
         <v>1.2941497598437599</v>
       </c>
-      <c r="G20" s="9">
+      <c r="G20" s="8">
         <v>0.54862180193228904</v>
       </c>
-      <c r="H20" s="9">
+      <c r="H20" s="8">
         <v>0.45957557872225802</v>
       </c>
-      <c r="I20" s="9">
+      <c r="I20" s="8">
         <v>0.16792711725721499</v>
       </c>
-      <c r="J20" s="9">
+      <c r="J20" s="8">
         <v>0.155525992178664</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="8">
         <v>0.123757319536642</v>
       </c>
-      <c r="L20" s="9">
+      <c r="L20" s="8">
         <v>3.7646701665883103E-2</v>
       </c>
     </row>
     <row r="21" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B21" s="8" t="s">
+      <c r="B21" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="10">
+      <c r="C21" s="9">
         <v>0.34647221226171099</v>
       </c>
-      <c r="D21" s="10">
+      <c r="D21" s="9">
         <v>0.20097472725941801</v>
       </c>
-      <c r="E21" s="10">
+      <c r="E21" s="9">
         <v>0.173832633365199</v>
       </c>
-      <c r="F21" s="10">
+      <c r="F21" s="9">
         <v>0.12941497598437601</v>
       </c>
-      <c r="G21" s="10">
+      <c r="G21" s="9">
         <v>5.4862180193228902E-2</v>
       </c>
-      <c r="H21" s="10">
+      <c r="H21" s="9">
         <v>4.5957557872225802E-2</v>
       </c>
-      <c r="I21" s="10">
+      <c r="I21" s="9">
         <v>1.6792711725721499E-2</v>
       </c>
-      <c r="J21" s="10">
+      <c r="J21" s="9">
         <v>1.5552599217866401E-2</v>
       </c>
-      <c r="K21" s="10">
+      <c r="K21" s="9">
         <v>1.2375731953664201E-2</v>
       </c>
-      <c r="L21" s="10">
+      <c r="L21" s="9">
         <v>3.7646701665883099E-3</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B22" s="8" t="s">
+      <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>0.34647221226171099</v>
       </c>
-      <c r="D22" s="10">
+      <c r="D22" s="9">
         <v>0.54744693952112899</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E22" s="9">
         <v>0.72127957288632794</v>
       </c>
-      <c r="F22" s="10">
+      <c r="F22" s="9">
         <v>0.85069454887070395</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="9">
         <v>0.90555672906393281</v>
       </c>
-      <c r="H22" s="10">
+      <c r="H22" s="9">
         <v>0.95151428693615858</v>
       </c>
-      <c r="I22" s="10">
+      <c r="I22" s="9">
         <v>0.96830699866188008</v>
       </c>
-      <c r="J22" s="10">
+      <c r="J22" s="9">
         <v>0.98385959787974653</v>
       </c>
-      <c r="K22" s="10">
+      <c r="K22" s="9">
         <v>0.99623532983341068</v>
       </c>
-      <c r="L22" s="11">
+      <c r="L22" s="10">
         <v>0.999999999999999</v>
       </c>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B23" s="17"/>
-      <c r="C23" s="18"/>
-      <c r="D23" s="18"/>
-      <c r="E23" s="18"/>
-      <c r="F23" s="18"/>
-      <c r="G23" s="18"/>
-      <c r="H23" s="18"/>
-      <c r="I23" s="18"/>
-      <c r="J23" s="18"/>
-      <c r="K23" s="18"/>
-      <c r="L23" s="18"/>
+      <c r="B23" s="16"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="17"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="17"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="17"/>
+      <c r="I23" s="17"/>
+      <c r="J23" s="17"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="17"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B24" s="8" t="s">
+      <c r="B24" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>1.2E-2</v>
       </c>
-      <c r="D24" s="9">
+      <c r="D24" s="8">
         <v>0.5</v>
       </c>
-      <c r="E24" s="9">
+      <c r="E24" s="8">
         <v>0.24099999999999999</v>
       </c>
-      <c r="F24" s="9">
+      <c r="F24" s="8">
         <v>-0.45300000000000001</v>
       </c>
-      <c r="G24" s="9">
+      <c r="G24" s="8">
         <v>-0.23200000000000001</v>
       </c>
-      <c r="H24" s="9">
+      <c r="H24" s="8">
         <v>0.34200000000000003</v>
       </c>
-      <c r="I24" s="9">
+      <c r="I24" s="8">
         <v>-0.13400000000000001</v>
       </c>
-      <c r="J24" s="9">
+      <c r="J24" s="8">
         <v>0.53</v>
       </c>
-      <c r="K24" s="9">
+      <c r="K24" s="8">
         <v>0.106</v>
       </c>
-      <c r="L24" s="9">
+      <c r="L24" s="8">
         <v>8.1000000000000003E-2</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B25" s="8" t="s">
+      <c r="B25" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="D25" s="9">
+      <c r="D25" s="8">
         <v>-0.11799999999999999</v>
       </c>
-      <c r="E25" s="9">
+      <c r="E25" s="8">
         <v>3.1E-2</v>
       </c>
-      <c r="F25" s="9">
+      <c r="F25" s="8">
         <v>0.17299999999999999</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="8">
         <v>-0.17599999999999999</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="8">
         <v>0.217</v>
       </c>
-      <c r="I25" s="9">
+      <c r="I25" s="8">
         <v>-0.505</v>
       </c>
-      <c r="J25" s="9">
+      <c r="J25" s="8">
         <v>-0.20200000000000001</v>
       </c>
-      <c r="K25" s="9">
+      <c r="K25" s="8">
         <v>0.59099999999999997</v>
       </c>
-      <c r="L25" s="9">
+      <c r="L25" s="8">
         <v>-2.9000000000000001E-2</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B26" s="8" t="s">
+      <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="9">
+      <c r="C26" s="8">
         <v>-0.438</v>
       </c>
-      <c r="D26" s="9">
+      <c r="D26" s="8">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="E26" s="9">
+      <c r="E26" s="8">
         <v>0.24</v>
       </c>
-      <c r="F26" s="9">
+      <c r="F26" s="8">
         <v>1.7000000000000001E-2</v>
       </c>
-      <c r="G26" s="9">
+      <c r="G26" s="8">
         <v>0.34</v>
       </c>
-      <c r="H26" s="9">
+      <c r="H26" s="8">
         <v>0.51800000000000002</v>
       </c>
-      <c r="I26" s="9">
+      <c r="I26" s="8">
         <v>0.30199999999999999</v>
       </c>
-      <c r="J26" s="9">
+      <c r="J26" s="8">
         <v>-0.153</v>
       </c>
-      <c r="K26" s="9">
+      <c r="K26" s="8">
         <v>-0.26200000000000001</v>
       </c>
-      <c r="L26" s="9">
+      <c r="L26" s="8">
         <v>-0.42</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B27" s="8" t="s">
+      <c r="B27" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C27" s="9">
+      <c r="C27" s="8">
         <v>0.24299999999999999</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="E27" s="9">
+      <c r="E27" s="8">
         <v>0.155</v>
       </c>
-      <c r="F27" s="9">
+      <c r="F27" s="8">
         <v>-5.3999999999999999E-2</v>
       </c>
-      <c r="G27" s="9">
+      <c r="G27" s="8">
         <v>0.01</v>
       </c>
-      <c r="H27" s="9">
+      <c r="H27" s="8">
         <v>-0.26500000000000001</v>
       </c>
-      <c r="I27" s="9">
+      <c r="I27" s="8">
         <v>-0.33</v>
       </c>
-      <c r="J27" s="9">
+      <c r="J27" s="8">
         <v>-0.496</v>
       </c>
-      <c r="K27" s="9">
+      <c r="K27" s="8">
         <v>-5.1999999999999998E-2</v>
       </c>
-      <c r="L27" s="9">
+      <c r="L27" s="8">
         <v>-0.4</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B28" s="8" t="s">
+      <c r="B28" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C28" s="9">
+      <c r="C28" s="8">
         <v>-0.46</v>
       </c>
-      <c r="D28" s="9">
+      <c r="D28" s="8">
         <v>0.19700000000000001</v>
       </c>
-      <c r="E28" s="9">
+      <c r="E28" s="8">
         <v>-1E-3</v>
       </c>
-      <c r="F28" s="9">
+      <c r="F28" s="8">
         <v>0.11</v>
       </c>
-      <c r="G28" s="9">
+      <c r="G28" s="8">
         <v>0.36</v>
       </c>
-      <c r="H28" s="9">
+      <c r="H28" s="8">
         <v>-0.28899999999999998</v>
       </c>
-      <c r="I28" s="9">
+      <c r="I28" s="8">
         <v>-0.42099999999999999</v>
       </c>
-      <c r="J28" s="9">
+      <c r="J28" s="8">
         <v>0.189</v>
       </c>
-      <c r="K28" s="9">
+      <c r="K28" s="8">
         <v>-0.43099999999999999</v>
       </c>
-      <c r="L28" s="9">
+      <c r="L28" s="8">
         <v>0.35399999999999998</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B29" s="8" t="s">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C29" s="9">
+      <c r="C29" s="8">
         <v>0.19800000000000001</v>
       </c>
-      <c r="D29" s="9">
+      <c r="D29" s="8">
         <v>0.21199999999999999</v>
       </c>
-      <c r="E29" s="9">
+      <c r="E29" s="8">
         <v>0.502</v>
       </c>
-      <c r="F29" s="9">
+      <c r="F29" s="8">
         <v>0.39500000000000002</v>
       </c>
-      <c r="G29" s="9">
+      <c r="G29" s="8">
         <v>0.42299999999999999</v>
       </c>
-      <c r="H29" s="9">
+      <c r="H29" s="8">
         <v>-4.1000000000000002E-2</v>
       </c>
-      <c r="I29" s="9">
+      <c r="I29" s="8">
         <v>0.224</v>
       </c>
-      <c r="J29" s="9">
+      <c r="J29" s="8">
         <v>0.04</v>
       </c>
-      <c r="K29" s="9">
+      <c r="K29" s="8">
         <v>0.42099999999999999</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="8">
         <v>0.313</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B30" s="8" t="s">
+      <c r="B30" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="9">
+      <c r="C30" s="8">
         <v>0.26300000000000001</v>
       </c>
-      <c r="D30" s="9">
+      <c r="D30" s="8">
         <v>-0.318</v>
       </c>
-      <c r="E30" s="9">
+      <c r="E30" s="8">
         <v>0.501</v>
       </c>
-      <c r="F30" s="9">
+      <c r="F30" s="8">
         <v>-1.4999999999999999E-2</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="8">
         <v>-0.19600000000000001</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="8">
         <v>0.32900000000000001</v>
       </c>
-      <c r="I30" s="9">
+      <c r="I30" s="8">
         <v>-0.29199999999999998</v>
       </c>
-      <c r="J30" s="9">
+      <c r="J30" s="8">
         <v>-0.29399999999999998</v>
       </c>
-      <c r="K30" s="9">
+      <c r="K30" s="8">
         <v>-0.38500000000000001</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="8">
         <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B31" s="8" t="s">
+      <c r="B31" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="8">
         <v>0.34499999999999997</v>
       </c>
-      <c r="D31" s="9">
+      <c r="D31" s="8">
         <v>-7.9817739316287994E-3</v>
       </c>
-      <c r="E31" s="9">
+      <c r="E31" s="8">
         <v>-0.16674029355220099</v>
       </c>
-      <c r="F31" s="12" t="s">
+      <c r="F31" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G31" s="9">
+      <c r="G31" s="8">
         <v>5.3848795797818698E-2</v>
       </c>
-      <c r="H31" s="9">
+      <c r="H31" s="8">
         <v>0.285356763811217</v>
       </c>
-      <c r="I31" s="9">
+      <c r="I31" s="8">
         <v>-0.33978239884967698</v>
       </c>
-      <c r="J31" s="9">
+      <c r="J31" s="8">
         <v>0.41138257293087199</v>
       </c>
-      <c r="K31" s="9">
+      <c r="K31" s="8">
         <v>-0.13935084873821499</v>
       </c>
-      <c r="L31" s="9">
+      <c r="L31" s="8">
         <v>-0.34553032137405598</v>
       </c>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B32" s="8" t="s">
+      <c r="B32" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="9">
+      <c r="C32" s="8">
         <v>-0.24719567089862399</v>
       </c>
-      <c r="D32" s="9">
+      <c r="D32" s="8">
         <v>0.31080674931020003</v>
       </c>
-      <c r="E32" s="9">
+      <c r="E32" s="8">
         <v>8.3604958564878498E-2</v>
       </c>
-      <c r="F32" s="9">
+      <c r="F32" s="8">
         <v>0.49636190281855702</v>
       </c>
-      <c r="G32" s="9">
+      <c r="G32" s="8">
         <v>-0.65886406267940201</v>
       </c>
-      <c r="H32" s="9">
+      <c r="H32" s="8">
         <v>-8.5305242651134594E-2</v>
       </c>
-      <c r="I32" s="9">
+      <c r="I32" s="8">
         <v>0.31275915359950002</v>
       </c>
-      <c r="J32" s="9">
+      <c r="J32" s="8">
         <v>-3.3558390830539603E-2</v>
       </c>
-      <c r="K32" s="9">
+      <c r="K32" s="8">
         <v>-0.193140930636652</v>
       </c>
-      <c r="L32" s="9">
+      <c r="L32" s="8">
         <v>0.10631005055559201</v>
       </c>
     </row>
     <row r="33" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="14">
         <v>0.130521587807608</v>
       </c>
-      <c r="D33" s="15">
+      <c r="D33" s="14">
         <v>0.35081842802783803</v>
       </c>
-      <c r="E33" s="16" t="s">
+      <c r="E33" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="F33" s="15">
+      <c r="F33" s="14">
         <v>4.61061787801373E-2</v>
       </c>
-      <c r="G33" s="15">
+      <c r="G33" s="14">
         <v>0.125967724313192</v>
       </c>
-      <c r="H33" s="15">
+      <c r="H33" s="14">
         <v>0.46388465752256802</v>
       </c>
-      <c r="I33" s="15">
+      <c r="I33" s="14">
         <v>4.0008113789061099E-2</v>
       </c>
-      <c r="J33" s="15">
+      <c r="J33" s="14">
         <v>-0.33730617189997703</v>
       </c>
-      <c r="K33" s="15">
+      <c r="K33" s="14">
         <v>-4.24552825242966E-4</v>
       </c>
-      <c r="L33" s="15">
+      <c r="L33" s="14">
         <v>0.43617274184920402</v>
       </c>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.35">
-      <c r="B34" s="20" t="s">
+      <c r="B34" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="20"/>
-      <c r="E34" s="20"/>
-      <c r="F34" s="20"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="6"/>
+      <c r="H34" s="6"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="6"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="6"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.35">
       <c r="B35" s="1"/>

</xml_diff>